<commit_message>
01.06.19 Today Last sales Updated 12:26am
</commit_message>
<xml_diff>
--- a/May/Daily Sales Info/All Details/31.05.19/DSR Wise Sales Report.xlsx
+++ b/May/Daily Sales Info/All Details/31.05.19/DSR Wise Sales Report.xlsx
@@ -52,7 +52,7 @@
     <t>-------------------------------------------------------</t>
   </si>
   <si>
-    <t>Date:30.05.19</t>
+    <t>Date:31.05.19</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,13 +557,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>158200</v>
+        <v>86545</v>
       </c>
       <c r="C6" s="2">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -571,13 +571,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>108630</v>
+        <v>31820</v>
       </c>
       <c r="C7" s="2">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -585,13 +585,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>115480</v>
+        <v>94660</v>
       </c>
       <c r="C8" s="2">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D8" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="9" customHeight="1">
@@ -608,15 +608,15 @@
       </c>
       <c r="B10" s="4">
         <f>SUM(B6:B8)</f>
-        <v>382310</v>
+        <v>213025</v>
       </c>
       <c r="C10" s="4">
         <f>SUM(C6:C8)</f>
-        <v>237</v>
+        <v>155</v>
       </c>
       <c r="D10" s="4">
         <f>SUM(D6:D8)</f>
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>